<commit_message>
Remove constants. Update docs
</commit_message>
<xml_diff>
--- a/doc/SheetsCounter.xlsx
+++ b/doc/SheetsCounter.xlsx
@@ -438,11 +438,11 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -472,11 +472,11 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6">
         <f t="shared" ref="B6:C6" si="1">+SUM(B2:B5)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="D6">
         <f>+SUM(D2:D5)</f>

</xml_diff>